<commit_message>
update exel delete jpeg
</commit_message>
<xml_diff>
--- a/дз9.xlsx
+++ b/дз9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenashevchenko/Desktop/айти марафон/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenashevchenko/Documents/GitHub/Lesson22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB27C37F-89B2-E440-A8AC-FBEFF4D8D6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF14C9E-B554-AC4B-AC9E-FA8CF22ED0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pairwise" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="15">
   <si>
     <t>Район</t>
   </si>
@@ -100,7 +100,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -123,11 +123,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,6 +157,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -448,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF8B3A0-ED97-F548-BF71-82C95A15CA3C}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -595,106 +621,63 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>